<commit_message>
Fixed CSV for #3 - partial matching might be added later in case it becomes an issue.
</commit_message>
<xml_diff>
--- a/Riddles/external_files/riddles_excel.xlsx
+++ b/Riddles/external_files/riddles_excel.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godof\Downloads\riddles-main\riddles-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Streaming\Scripts &amp; Codes\cs_codes\Riddles\external_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{95018F7C-ACB0-4485-B2AC-0EC88738DEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9BB0F7-CCB0-4A8F-897B-785C307C2EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="8490" yWindow="600" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="riddles" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">riddles!$A$1:$H$378</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">riddles!$A$1:$H$377</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="1257">
   <si>
     <t>ANSWERS</t>
   </si>
@@ -3703,18 +3703,12 @@
     <t xml:space="preserve"> yet the strongest man can't hold me for more than 5 minutes. What am I?</t>
   </si>
   <si>
-    <t>Breath.</t>
-  </si>
-  <si>
     <t>What goes in the water black and comes out red?</t>
   </si>
   <si>
     <t>What two things can you never eat for breakfast?</t>
   </si>
   <si>
-    <t>Lunch and dinner.</t>
-  </si>
-  <si>
     <t>What is brown and sticky?</t>
   </si>
   <si>
@@ -3730,15 +3724,6 @@
     <t>I occur once in a minute...</t>
   </si>
   <si>
-    <t>The letter 'm'</t>
-  </si>
-  <si>
-    <t>What is the difference between a grandmother and a granary?</t>
-  </si>
-  <si>
-    <t>one is one's born-kin, the other is one's corn-bin</t>
-  </si>
-  <si>
     <t>I pass before the sun</t>
   </si>
   <si>
@@ -3803,12 +3788,18 @@
   </si>
   <si>
     <t>QUESTIONS - 7</t>
+  </si>
+  <si>
+    <t>Lunch and dinner</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4641,47 +4632,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="67.85546875" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="F1" t="s">
         <v>1253</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>1254</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1255</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1258</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1259</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -6389,16 +6381,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1244</v>
+        <v>1239</v>
       </c>
       <c r="B93" t="s">
-        <v>1245</v>
+        <v>1240</v>
       </c>
       <c r="C93" t="s">
-        <v>1246</v>
+        <v>1241</v>
       </c>
       <c r="H93" t="s">
-        <v>1247</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -7403,7 +7395,7 @@
         <v>1177</v>
       </c>
       <c r="H165" t="s">
-        <v>1252</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7540,13 +7532,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
       <c r="B178" t="s">
-        <v>1242</v>
+        <v>1237</v>
       </c>
       <c r="H178" t="s">
-        <v>1243</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -7606,13 +7598,13 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>1238</v>
+        <v>1233</v>
       </c>
       <c r="B184" t="s">
-        <v>1239</v>
+        <v>1234</v>
       </c>
       <c r="H184" t="s">
-        <v>1240</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -8426,7 +8418,7 @@
         <v>1225</v>
       </c>
       <c r="H258" t="s">
-        <v>1226</v>
+        <v>563</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -8699,10 +8691,10 @@
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="H291" t="s">
-        <v>1235</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.25">
@@ -9043,7 +9035,7 @@
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="H334" t="s">
         <v>1029</v>
@@ -9051,10 +9043,10 @@
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="H335" t="s">
-        <v>1248</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.25">
@@ -9147,10 +9139,10 @@
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H347" t="s">
-        <v>1249</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.25">
@@ -9211,10 +9203,10 @@
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="H355" t="s">
-        <v>1251</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.25">
@@ -9243,168 +9235,161 @@
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>1236</v>
+        <v>1156</v>
       </c>
       <c r="H359" t="s">
-        <v>1237</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1156</v>
+        <v>655</v>
       </c>
       <c r="H360" t="s">
-        <v>1157</v>
+        <v>656</v>
       </c>
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>655</v>
+        <v>385</v>
       </c>
       <c r="H361" t="s">
-        <v>656</v>
+        <v>386</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>385</v>
+        <v>149</v>
       </c>
       <c r="H362" t="s">
-        <v>386</v>
+        <v>150</v>
       </c>
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>149</v>
+        <v>1230</v>
       </c>
       <c r="H363" t="s">
-        <v>150</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>1232</v>
+        <v>86</v>
       </c>
       <c r="H364" t="s">
-        <v>1250</v>
+        <v>87</v>
       </c>
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>86</v>
+        <v>746</v>
       </c>
       <c r="H365" t="s">
-        <v>87</v>
+        <v>747</v>
       </c>
     </row>
     <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>746</v>
+        <v>27</v>
       </c>
       <c r="H366" t="s">
-        <v>747</v>
+        <v>28</v>
       </c>
     </row>
     <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>27</v>
+        <v>1031</v>
       </c>
       <c r="H367" t="s">
-        <v>28</v>
+        <v>402</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>1031</v>
+        <v>1227</v>
       </c>
       <c r="H368" t="s">
-        <v>402</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>1228</v>
+        <v>949</v>
       </c>
       <c r="H369" t="s">
-        <v>1229</v>
+        <v>950</v>
       </c>
     </row>
     <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>949</v>
+        <v>247</v>
       </c>
       <c r="H370" t="s">
-        <v>950</v>
+        <v>248</v>
       </c>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>247</v>
+        <v>604</v>
       </c>
       <c r="H371" t="s">
-        <v>248</v>
+        <v>605</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>604</v>
+        <v>751</v>
       </c>
       <c r="H372" t="s">
-        <v>605</v>
+        <v>752</v>
       </c>
     </row>
     <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="H373" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>749</v>
+        <v>1199</v>
       </c>
       <c r="H374" t="s">
-        <v>750</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>1199</v>
+        <v>992</v>
       </c>
       <c r="H375" t="s">
-        <v>1200</v>
+        <v>640</v>
       </c>
     </row>
     <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>992</v>
+        <v>1020</v>
       </c>
       <c r="H376" t="s">
-        <v>640</v>
+        <v>315</v>
       </c>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>1020</v>
+        <v>807</v>
       </c>
       <c r="H377" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
-        <v>807</v>
-      </c>
-      <c r="H378" t="s">
         <v>470</v>
       </c>
     </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:H378">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H378">
-      <sortCondition ref="G1:G378"/>
+  <autoFilter ref="A1:H377" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H377">
+      <sortCondition ref="G1:G377"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>